<commit_message>
Adding more experiments adding more hidden layers (hidden_dim =100, 300, 600)
</commit_message>
<xml_diff>
--- a/experiments_colors.xlsx
+++ b/experiments_colors.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\vicaran93\repos\AI-certificate-stanford\CS224\cs224u\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{947B9655-A9E7-423F-A241-5E06B5360EC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B11F0F88-340E-4DAD-97A6-3955DCCF9C55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{5FFEFC4F-FE0E-4623-8954-E4468EA0D732}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Experiment</t>
   </si>
@@ -70,7 +70,19 @@
     <t>Baseline with dev_mod based on whitspace tokenization and colors represented by fourier transform</t>
   </si>
   <si>
-    <t>Based on experiment 1 + ColorizedInputDescriber</t>
+    <t>RNN 3 layers encoder/decoder</t>
+  </si>
+  <si>
+    <t>LSTM 1 layer</t>
+  </si>
+  <si>
+    <t>Based on experiment 1 + ColorizedInputDescriber (targets added to embeddings)</t>
+  </si>
+  <si>
+    <t>LSTM 1 layer + hidden_dim=100</t>
+  </si>
+  <si>
+    <t>LSTM 1 layer + hidden_dim=300</t>
   </si>
 </sst>
 </file>
@@ -422,17 +434,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73F86C07-C85B-46FE-900B-83A0B1CE959C}">
-  <dimension ref="B1:E11"/>
+  <dimension ref="B1:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="15.6328125" customWidth="1"/>
     <col min="3" max="3" width="20.6328125" customWidth="1"/>
-    <col min="4" max="4" width="15.6328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.26953125" customWidth="1"/>
     <col min="5" max="5" width="85.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -452,138 +464,194 @@
     </row>
     <row r="2" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B2">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="C2">
-        <v>0.80362798733083696</v>
+        <v>0.80996256838468095</v>
       </c>
       <c r="D2">
-        <v>0.63070894471692196</v>
+        <v>0.63218752740925699</v>
       </c>
       <c r="E2" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B3">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="C3">
-        <v>0.79556579326230903</v>
+        <v>0.80881082637489199</v>
       </c>
       <c r="D3">
-        <v>0.65917977999260302</v>
+        <v>0.63343120661934904</v>
       </c>
       <c r="E3" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B4">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C4">
-        <v>0.79009501871580701</v>
+        <v>0.80362798733083696</v>
       </c>
       <c r="D4">
-        <v>0.62904030780921905</v>
+        <v>0.63070894471692196</v>
       </c>
       <c r="E4" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B5">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C5">
-        <v>0.77828966311546199</v>
+        <v>0.79671753527209899</v>
       </c>
       <c r="D5">
-        <v>0.65715647832434898</v>
+        <v>0.62949904887654395</v>
+      </c>
+      <c r="E5" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B6">
-        <v>0.1</v>
+        <v>3</v>
       </c>
       <c r="C6">
-        <v>0.76418082349553695</v>
+        <v>0.79556579326230903</v>
       </c>
       <c r="D6">
-        <v>0.67793927924818198</v>
+        <v>0.65917977999260302</v>
       </c>
       <c r="E6" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B7">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="C7">
-        <v>0.75755830693924497</v>
+        <v>0.79527785775986104</v>
       </c>
       <c r="D7">
-        <v>0.62214012836330002</v>
+        <v>0.63325507730990904</v>
       </c>
       <c r="E7" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B8">
+        <v>5</v>
+      </c>
+      <c r="C8">
+        <v>0.79009501871580701</v>
+      </c>
+      <c r="D8">
+        <v>0.62904030780921905</v>
+      </c>
+      <c r="E8" t="s">
         <v>4</v>
-      </c>
-      <c r="C8">
-        <v>0.689893463864094</v>
-      </c>
-      <c r="D8">
-        <v>0.70707360247984596</v>
       </c>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B9">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C9">
-        <v>0.68931759285919902</v>
+        <v>0.77828966311546199</v>
       </c>
       <c r="D9">
-        <v>0.70697763700930905</v>
+        <v>0.65715647832434898</v>
       </c>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B10">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="C10">
-        <v>0.399654477397063</v>
+        <v>0.76418082349553695</v>
       </c>
       <c r="D10">
-        <v>5.7112006910451998E-2</v>
+        <v>0.67793927924818198</v>
       </c>
       <c r="E10" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B11">
+        <v>2</v>
+      </c>
+      <c r="C11">
+        <v>0.75755830693924497</v>
+      </c>
+      <c r="D11">
+        <v>0.62214012836330002</v>
+      </c>
+      <c r="E11" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B12">
+        <v>4</v>
+      </c>
+      <c r="C12">
+        <v>0.689893463864094</v>
+      </c>
+      <c r="D12">
+        <v>0.70707360247984596</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B13">
+        <v>7</v>
+      </c>
+      <c r="C13">
+        <v>0.68931759285919902</v>
+      </c>
+      <c r="D13">
+        <v>0.70697763700930905</v>
+      </c>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B14">
+        <v>0</v>
+      </c>
+      <c r="C14">
+        <v>0.399654477397063</v>
+      </c>
+      <c r="D14">
+        <v>5.7112006910451998E-2</v>
+      </c>
+      <c r="E14" t="s">
         <v>8</v>
       </c>
-      <c r="C11">
-        <v>0.80881082637489199</v>
-      </c>
-      <c r="D11">
-        <v>0.63343120661934904</v>
-      </c>
-      <c r="E11" t="s">
-        <v>10</v>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B15">
+        <v>11</v>
+      </c>
+      <c r="C15">
+        <v>0.81341779441405104</v>
+      </c>
+      <c r="D15">
+        <v>0.63137915035306502</v>
+      </c>
+      <c r="E15" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="B1:E1" xr:uid="{73F86C07-C85B-46FE-900B-83A0B1CE959C}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:E10">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:E14">
       <sortCondition descending="1" ref="C1"/>
     </sortState>
   </autoFilter>

</xml_diff>